<commit_message>
#register #login v1 #theater play v1
</commit_message>
<xml_diff>
--- a/Documents/Timesheet.xlsx
+++ b/Documents/Timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -92,10 +92,28 @@
     <t>impl hibernate model</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>16.04.2016</t>
+  </si>
+  <si>
+    <t>impl message properties</t>
+  </si>
+  <si>
+    <t>template.jsp</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>Theater/play simple</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>18.04.2016</t>
+  </si>
+  <si>
+    <t>Inprocess</t>
   </si>
 </sst>
 </file>
@@ -472,7 +490,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,7 +610,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(C:C,C1)</f>
-        <v>21.5</v>
+        <v>29.2</v>
       </c>
       <c r="K5" t="s">
         <v>16</v>
@@ -612,7 +630,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>8</v>
@@ -629,10 +647,10 @@
         <v>0.5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
@@ -646,58 +664,115 @@
         <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -845,7 +920,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576 F1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
       <formula1>"Pending,Inprocess, Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>